<commit_message>
Endlich fertig ALLA. EHRE IN DEN ARSCH
</commit_message>
<xml_diff>
--- a/Versuch-3-2_pn_Uebergang_und_Solarzelle/Versuchsdaten/Messwerte.xlsx
+++ b/Versuch-3-2_pn_Uebergang_und_Solarzelle/Versuchsdaten/Messwerte.xlsx
@@ -8,22 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benny\git\Ausarbeitungen_Physikpraktikum_SoSe2022\Versuch-3-2_pn_Uebergang_und_Solarzelle\Versuchsdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CE8670-A3D9-4FE5-8829-79E436D99290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE4A2EE-9376-42C9-AD25-8F288860E563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20596" windowHeight="14378" activeTab="1" xr2:uid="{D4DF9782-D38F-422E-89AA-7C82959997A6}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="1" xr2:uid="{D4DF9782-D38F-422E-89AA-7C82959997A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Teil A Diode unbeleuchtet" sheetId="1" r:id="rId1"/>
     <sheet name="Teil B Solarzelle" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Teil A Diode unbeleuchtet'!$C$6:$C$67</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Teil A Diode unbeleuchtet'!$D$5</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Teil A Diode unbeleuchtet'!$D$6:$D$67</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Teil A Diode unbeleuchtet'!$C$6:$C$67</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Teil A Diode unbeleuchtet'!$D$5</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Teil A Diode unbeleuchtet'!$D$6:$D$67</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
   <si>
     <t>Ud</t>
   </si>
@@ -71,6 +63,15 @@
   </si>
   <si>
     <t>mm^2</t>
+  </si>
+  <si>
+    <t>Pmax</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -103,7 +104,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -176,11 +177,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -214,6 +263,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -245,37 +309,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -305,17 +339,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="x"/>
-            <c:size val="2"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -724,18 +748,75 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Strom</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> [A]</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -764,13 +845,14 @@
         <c:crossAx val="1457912463"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
-        <c:minorUnit val="1"/>
+        <c:majorUnit val="0.25"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1457912463"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.1"/>
+          <c:min val="-2.0000000000000004E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -788,18 +870,75 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Spannung</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> [V]</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -888,39 +1027,96 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>P_max</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Teil B Solarzelle'!$K$6:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Teil B Solarzelle'!$L$6:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-5.7847000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5.7847000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.7847000000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-55F0-4DCE-9ED9-9BBDDE913EBB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1457903311"/>
+        <c:axId val="1457912463"/>
+      </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -948,17 +1144,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="x"/>
-            <c:size val="2"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1199,18 +1385,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Strom [A]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1239,13 +1477,15 @@
         <c:crossAx val="1457912463"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
-        <c:minorUnit val="1"/>
+        <c:majorUnit val="0.25"/>
+        <c:minorUnit val="0.25"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1457912463"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5.000000000000001E-2"/>
+          <c:min val="-7.0000000000000007E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1263,18 +1503,83 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Spannung</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> [V]</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.8654540529853582E-3"/>
+              <c:y val="0.32649703237938532"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1312,6 +1617,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2471,10 +2807,10 @@
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>100012</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>226017</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>121080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2507,15 +2843,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>150018</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:colOff>711993</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>100012</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2842,16 +3178,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B997AB-B6B6-4DF8-8244-DE8B156C1245}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="C4:J67"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="5" spans="3:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="7" t="s">
         <v>0</v>
       </c>
@@ -2862,7 +3201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" s="9">
         <v>-2</v>
       </c>
@@ -2874,12 +3213,12 @@
         <v>-4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" s="11">
         <v>-1</v>
       </c>
       <c r="D7" s="12">
-        <f>E7/150</f>
+        <f t="shared" ref="D7:D37" si="0">E7/150</f>
         <v>-1.0666666666666667E-4</v>
       </c>
       <c r="E7" s="11">
@@ -2889,12 +3228,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" s="11">
         <v>0</v>
       </c>
       <c r="D8" s="12">
-        <f>E8/150</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E8" s="11">
@@ -2907,12 +3246,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="11">
         <v>0.02</v>
       </c>
       <c r="D9" s="12">
-        <f>E9/150</f>
+        <f t="shared" si="0"/>
         <v>4.2000000000000004E-6</v>
       </c>
       <c r="E9" s="11">
@@ -2922,12 +3261,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C10" s="11">
         <v>0.03</v>
       </c>
       <c r="D10" s="12">
-        <f>E10/150</f>
+        <f t="shared" si="0"/>
         <v>6.8666666666666673E-6</v>
       </c>
       <c r="E10" s="11">
@@ -2944,552 +3283,552 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11" s="11">
         <v>0.04</v>
       </c>
       <c r="D11" s="12">
-        <f>E11/150</f>
+        <f t="shared" si="0"/>
         <v>9.5333333333333341E-6</v>
       </c>
       <c r="E11" s="11">
         <v>1.4300000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C12" s="11">
         <v>0.05</v>
       </c>
       <c r="D12" s="12">
-        <f>E12/150</f>
+        <f t="shared" si="0"/>
         <v>1.2933333333333334E-5</v>
       </c>
       <c r="E12" s="11">
         <v>1.9400000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C13" s="11">
         <v>0.06</v>
       </c>
       <c r="D13" s="12">
-        <f>E13/150</f>
+        <f t="shared" si="0"/>
         <v>1.6333333333333332E-5</v>
       </c>
       <c r="E13" s="11">
         <v>2.4499999999999999E-3</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C14" s="11">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D14" s="12">
-        <f>E14/150</f>
+        <f t="shared" si="0"/>
         <v>2.0666666666666666E-5</v>
       </c>
       <c r="E14" s="11">
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C15" s="11">
         <v>0.08</v>
       </c>
       <c r="D15" s="12">
-        <f>E15/150</f>
+        <f t="shared" si="0"/>
         <v>2.5666666666666666E-5</v>
       </c>
       <c r="E15" s="11">
         <v>3.8500000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C16" s="11">
         <v>0.09</v>
       </c>
       <c r="D16" s="12">
-        <f>E16/150</f>
+        <f t="shared" si="0"/>
         <v>3.1133333333333329E-5</v>
       </c>
       <c r="E16" s="11">
         <v>4.6699999999999997E-3</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" s="11">
         <v>0.1</v>
       </c>
       <c r="D17" s="12">
-        <f>E17/150</f>
+        <f t="shared" si="0"/>
         <v>3.7400000000000001E-5</v>
       </c>
       <c r="E17" s="11">
         <v>5.6100000000000004E-3</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" s="11">
         <v>0.11</v>
       </c>
       <c r="D18" s="12">
-        <f>E18/150</f>
+        <f t="shared" si="0"/>
         <v>4.4466666666666666E-5</v>
       </c>
       <c r="E18" s="11">
         <v>6.6699999999999997E-3</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" s="11">
         <v>0.12</v>
       </c>
       <c r="D19" s="12">
-        <f>E19/150</f>
+        <f t="shared" si="0"/>
         <v>5.2333333333333329E-5</v>
       </c>
       <c r="E19" s="11">
         <v>7.8499999999999993E-3</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C20" s="11">
         <v>0.13</v>
       </c>
       <c r="D20" s="12">
-        <f>E20/150</f>
+        <f t="shared" si="0"/>
         <v>6.120000000000001E-5</v>
       </c>
       <c r="E20" s="11">
         <v>9.1800000000000007E-3</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" s="11">
         <v>0.14000000000000001</v>
       </c>
       <c r="D21" s="12">
-        <f>E21/150</f>
+        <f t="shared" si="0"/>
         <v>7.2133333333333329E-5</v>
       </c>
       <c r="E21" s="11">
         <v>1.082E-2</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C22" s="11">
         <v>0.15</v>
       </c>
       <c r="D22" s="12">
-        <f>E22/150</f>
+        <f t="shared" si="0"/>
         <v>8.2999999999999998E-5</v>
       </c>
       <c r="E22" s="11">
         <v>1.2449999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C23" s="11">
         <v>0.16</v>
       </c>
       <c r="D23" s="12">
-        <f>E23/150</f>
+        <f t="shared" si="0"/>
         <v>9.7E-5</v>
       </c>
       <c r="E23" s="11">
         <v>1.455E-2</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C24" s="11">
         <v>0.17</v>
       </c>
       <c r="D24" s="12">
-        <f>E24/150</f>
+        <f t="shared" si="0"/>
         <v>1.1186666666666667E-4</v>
       </c>
       <c r="E24" s="11">
         <v>1.678E-2</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C25" s="11">
         <v>0.18</v>
       </c>
       <c r="D25" s="12">
-        <f>E25/150</f>
+        <f t="shared" si="0"/>
         <v>1.282E-4</v>
       </c>
       <c r="E25" s="11">
         <v>1.9230000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C26" s="11">
         <v>0.19</v>
       </c>
       <c r="D26" s="12">
-        <f>E26/150</f>
+        <f t="shared" si="0"/>
         <v>1.4860000000000001E-4</v>
       </c>
       <c r="E26" s="11">
         <v>2.2290000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C27" s="11">
         <v>0.2</v>
       </c>
       <c r="D27" s="12">
-        <f>E27/150</f>
+        <f t="shared" si="0"/>
         <v>1.6999999999999999E-4</v>
       </c>
       <c r="E27" s="11">
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C28" s="11">
         <v>0.21</v>
       </c>
       <c r="D28" s="12">
-        <f>E28/150</f>
+        <f t="shared" si="0"/>
         <v>1.9233333333333334E-4</v>
       </c>
       <c r="E28" s="11">
         <v>2.8850000000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C29" s="11">
         <v>0.22</v>
       </c>
       <c r="D29" s="12">
-        <f>E29/150</f>
+        <f t="shared" si="0"/>
         <v>2.2000000000000001E-4</v>
       </c>
       <c r="E29" s="11">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C30" s="11">
         <v>0.23</v>
       </c>
       <c r="D30" s="12">
-        <f>E30/150</f>
+        <f t="shared" si="0"/>
         <v>2.5119999999999998E-4</v>
       </c>
       <c r="E30" s="11">
         <v>3.7679999999999998E-2</v>
       </c>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C31" s="11">
         <v>0.24</v>
       </c>
       <c r="D31" s="12">
-        <f>E31/150</f>
+        <f t="shared" si="0"/>
         <v>2.8486666666666663E-4</v>
       </c>
       <c r="E31" s="11">
         <v>4.2729999999999997E-2</v>
       </c>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C32" s="11">
         <v>0.25</v>
       </c>
       <c r="D32" s="12">
-        <f>E32/150</f>
+        <f t="shared" si="0"/>
         <v>3.2373333333333331E-4</v>
       </c>
       <c r="E32" s="11">
         <v>4.8559999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" s="11">
         <v>0.26</v>
       </c>
       <c r="D33" s="12">
-        <f>E33/150</f>
+        <f t="shared" si="0"/>
         <v>3.6913333333333333E-4</v>
       </c>
       <c r="E33" s="11">
         <v>5.5370000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C34" s="11">
         <v>0.27</v>
       </c>
       <c r="D34" s="12">
-        <f>E34/150</f>
+        <f t="shared" si="0"/>
         <v>4.2113333333333334E-4</v>
       </c>
       <c r="E34" s="11">
         <v>6.3170000000000004E-2</v>
       </c>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C35" s="11">
         <v>0.28000000000000003</v>
       </c>
       <c r="D35" s="12">
-        <f>E35/150</f>
+        <f t="shared" si="0"/>
         <v>4.7373333333333332E-4</v>
       </c>
       <c r="E35" s="11">
         <v>7.1059999999999998E-2</v>
       </c>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C36" s="11">
         <v>0.28999999999999998</v>
       </c>
       <c r="D36" s="12">
-        <f>E36/150</f>
+        <f t="shared" si="0"/>
         <v>5.4213333333333336E-4</v>
       </c>
       <c r="E36" s="11">
         <v>8.1320000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C37" s="11">
         <v>0.3</v>
       </c>
       <c r="D37" s="12">
-        <f>E37/150</f>
+        <f t="shared" si="0"/>
         <v>6.1233333333333333E-4</v>
       </c>
       <c r="E37" s="11">
         <v>9.1850000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C38" s="11">
         <v>0.31</v>
       </c>
       <c r="D38" s="12">
-        <f>E38/150</f>
+        <f t="shared" ref="D38:D56" si="1">E38/150</f>
         <v>6.9066666666666669E-4</v>
       </c>
       <c r="E38" s="11">
         <v>0.1036</v>
       </c>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C39" s="11">
         <v>0.32</v>
       </c>
       <c r="D39" s="12">
-        <f>E39/150</f>
+        <f t="shared" si="1"/>
         <v>7.8926666666666659E-4</v>
       </c>
       <c r="E39" s="11">
         <v>0.11839</v>
       </c>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C40" s="11">
         <v>0.33</v>
       </c>
       <c r="D40" s="12">
-        <f>E40/150</f>
+        <f t="shared" si="1"/>
         <v>9.1346666666666668E-4</v>
       </c>
       <c r="E40" s="11">
         <v>0.13702</v>
       </c>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C41" s="11">
         <v>0.34</v>
       </c>
       <c r="D41" s="12">
-        <f>E41/150</f>
+        <f t="shared" si="1"/>
         <v>1.0469333333333335E-3</v>
       </c>
       <c r="E41" s="11">
         <v>0.15704000000000001</v>
       </c>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C42" s="11">
         <v>0.35</v>
       </c>
       <c r="D42" s="12">
-        <f>E42/150</f>
+        <f t="shared" si="1"/>
         <v>1.2128666666666667E-3</v>
       </c>
       <c r="E42" s="11">
         <v>0.18193000000000001</v>
       </c>
     </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C43" s="11">
         <v>0.36</v>
       </c>
       <c r="D43" s="12">
-        <f>E43/150</f>
+        <f t="shared" si="1"/>
         <v>1.4013333333333334E-3</v>
       </c>
       <c r="E43" s="11">
         <v>0.2102</v>
       </c>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C44" s="11">
         <v>0.37</v>
       </c>
       <c r="D44" s="12">
-        <f>E44/150</f>
+        <f t="shared" si="1"/>
         <v>1.6366666666666667E-3</v>
       </c>
       <c r="E44" s="11">
         <v>0.2455</v>
       </c>
     </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C45" s="11">
         <v>0.38</v>
       </c>
       <c r="D45" s="12">
-        <f>E45/150</f>
+        <f t="shared" si="1"/>
         <v>1.9059999999999999E-3</v>
       </c>
       <c r="E45" s="11">
         <v>0.28589999999999999</v>
       </c>
     </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C46" s="11">
         <v>0.39</v>
       </c>
       <c r="D46" s="12">
-        <f>E46/150</f>
+        <f t="shared" si="1"/>
         <v>2.2400000000000002E-3</v>
       </c>
       <c r="E46" s="11">
         <v>0.33600000000000002</v>
       </c>
     </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C47" s="11">
         <v>0.4</v>
       </c>
       <c r="D47" s="12">
-        <f>E47/150</f>
+        <f t="shared" si="1"/>
         <v>2.6406666666666666E-3</v>
       </c>
       <c r="E47" s="11">
         <v>0.39610000000000001</v>
       </c>
     </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C48" s="11">
         <v>0.41</v>
       </c>
       <c r="D48" s="12">
-        <f>E48/150</f>
+        <f t="shared" si="1"/>
         <v>3.1699999999999996E-3</v>
       </c>
       <c r="E48" s="11">
         <v>0.47549999999999998</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="11">
         <v>0.42</v>
       </c>
       <c r="D49" s="12">
-        <f>E49/150</f>
+        <f t="shared" si="1"/>
         <v>3.7740000000000004E-3</v>
       </c>
       <c r="E49" s="11">
         <v>0.56610000000000005</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" s="11">
         <v>0.43</v>
       </c>
       <c r="D50" s="12">
-        <f>E50/150</f>
+        <f t="shared" si="1"/>
         <v>4.5713333333333335E-3</v>
       </c>
       <c r="E50" s="11">
         <v>0.68569999999999998</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C51" s="11">
         <v>0.44</v>
       </c>
       <c r="D51" s="12">
-        <f>E51/150</f>
+        <f t="shared" si="1"/>
         <v>5.6300000000000005E-3</v>
       </c>
       <c r="E51" s="11">
         <v>0.84450000000000003</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C52" s="11">
         <v>0.45</v>
       </c>
       <c r="D52" s="12">
-        <f>E52/150</f>
+        <f t="shared" si="1"/>
         <v>6.8339999999999989E-3</v>
       </c>
       <c r="E52" s="11">
         <v>1.0250999999999999</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C53" s="11">
         <v>0.46</v>
       </c>
       <c r="D53" s="12">
-        <f>E53/150</f>
+        <f t="shared" si="1"/>
         <v>8.3079999999999994E-3</v>
       </c>
       <c r="E53" s="11">
         <v>1.2462</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C54" s="11">
         <v>0.47</v>
       </c>
       <c r="D54" s="12">
-        <f>E54/150</f>
+        <f t="shared" si="1"/>
         <v>1.0368666666666667E-2</v>
       </c>
       <c r="E54" s="11">
         <v>1.5552999999999999</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C55" s="11">
         <v>0.48</v>
       </c>
       <c r="D55" s="12">
-        <f>E55/150</f>
+        <f t="shared" si="1"/>
         <v>1.3100000000000001E-2</v>
       </c>
       <c r="E55" s="11">
         <v>1.9650000000000001</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C56" s="11">
         <v>0.49</v>
       </c>
       <c r="D56" s="12">
-        <f>E56/150</f>
+        <f t="shared" si="1"/>
         <v>1.6633333333333333E-2</v>
       </c>
       <c r="E56" s="11">
@@ -3497,12 +3836,12 @@
       </c>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C57" s="11">
         <v>0.5</v>
       </c>
       <c r="D57" s="12">
-        <f t="shared" ref="D57:D67" si="0">E57/150</f>
+        <f t="shared" ref="D57:D63" si="2">E57/150</f>
         <v>2.104E-2</v>
       </c>
       <c r="E57" s="11">
@@ -3510,12 +3849,12 @@
       </c>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C58" s="11">
         <v>0.51</v>
       </c>
       <c r="D58" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.7493333333333331E-2</v>
       </c>
       <c r="E58" s="11">
@@ -3523,12 +3862,12 @@
       </c>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C59" s="11">
         <v>0.52</v>
       </c>
       <c r="D59" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.5026666666666664E-2</v>
       </c>
       <c r="E59" s="11">
@@ -3536,12 +3875,12 @@
       </c>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C60" s="11">
         <v>0.53</v>
       </c>
       <c r="D60" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.5419999999999995E-2</v>
       </c>
       <c r="E60" s="11">
@@ -3549,12 +3888,12 @@
       </c>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C61" s="11">
         <v>0.54</v>
       </c>
       <c r="D61" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.9006666666666673E-2</v>
       </c>
       <c r="E61" s="11">
@@ -3562,12 +3901,12 @@
       </c>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C62" s="11">
         <v>0.55000000000000004</v>
       </c>
       <c r="D62" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.6933333333333326E-2</v>
       </c>
       <c r="E62" s="11">
@@ -3575,12 +3914,12 @@
       </c>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C63" s="11">
         <v>0.56000000000000005</v>
       </c>
       <c r="D63" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.8853333333333335E-2</v>
       </c>
       <c r="E63" s="11">
@@ -3588,7 +3927,7 @@
       </c>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C64" s="11">
         <v>0.56999999999999995</v>
       </c>
@@ -3600,7 +3939,7 @@
       </c>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C65" s="11">
         <v>0.57999999999999996</v>
       </c>
@@ -3612,7 +3951,7 @@
       </c>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C66" s="11">
         <v>0.59</v>
       </c>
@@ -3624,7 +3963,7 @@
       </c>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C67" s="11">
         <v>0.6</v>
       </c>
@@ -3638,314 +3977,453 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="33" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E10BA3F0-FC29-43DC-B422-6AD0E722AD0D}">
-  <dimension ref="C4:H67"/>
+  <dimension ref="C4:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="H7:J10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="5" spans="3:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="F5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C6" s="9">
         <v>-2</v>
       </c>
       <c r="D6" s="10">
-        <f>E6/150</f>
+        <f t="shared" ref="D6:D36" si="0">E6/150</f>
         <v>-6.5000000000000002E-2</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="16">
         <v>-9.75</v>
       </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="F6" s="10">
+        <f>C6*D6</f>
+        <v>0.13</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>-5.7847000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C7" s="11">
         <v>-1</v>
       </c>
       <c r="D7" s="12">
-        <f>E7/150</f>
+        <f t="shared" si="0"/>
         <v>-6.5000000000000002E-2</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="17">
         <v>-9.75</v>
       </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="F7" s="10">
+        <f t="shared" ref="F7:F36" si="1">C7*D7</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C8" s="11">
         <v>0</v>
       </c>
       <c r="D8" s="12">
-        <f>E8/150</f>
+        <f t="shared" si="0"/>
         <v>-6.433333333333334E-2</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="17">
         <v>-9.65</v>
       </c>
+      <c r="F8" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="K8">
+        <v>0.42</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C9" s="11">
         <v>0.02</v>
       </c>
       <c r="D9" s="12">
-        <f>E9/150</f>
+        <f t="shared" si="0"/>
         <v>-6.3933333333333328E-2</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="17">
         <v>-9.59</v>
       </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="F9" s="10">
+        <f t="shared" si="1"/>
+        <v>-1.2786666666666667E-3</v>
+      </c>
+      <c r="K9">
+        <v>0.42</v>
+      </c>
+      <c r="L9">
+        <v>-5.7847000000000003E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C10" s="11">
         <v>0.04</v>
       </c>
       <c r="D10" s="12">
-        <f>E10/150</f>
+        <f t="shared" si="0"/>
         <v>-6.4093333333333335E-2</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="17">
         <v>-9.6140000000000008</v>
       </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="F10" s="10">
+        <f t="shared" si="1"/>
+        <v>-2.5637333333333335E-3</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>-5.7847000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C11" s="11">
         <v>0.06</v>
       </c>
       <c r="D11" s="12">
-        <f>E11/150</f>
+        <f t="shared" si="0"/>
         <v>-6.386E-2</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="17">
         <v>-9.5790000000000006</v>
       </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="F11" s="10">
+        <f t="shared" si="1"/>
+        <v>-3.8315999999999997E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C12" s="11">
         <v>0.08</v>
       </c>
       <c r="D12" s="12">
-        <f>E12/150</f>
+        <f t="shared" si="0"/>
         <v>-6.3933333333333328E-2</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="17">
         <v>-9.59</v>
       </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="F12" s="10">
+        <f t="shared" si="1"/>
+        <v>-5.1146666666666667E-3</v>
+      </c>
+      <c r="H12">
+        <f>(F29)/(C34*D8)</f>
+        <v>0.72625348744519713</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C13" s="11">
         <v>0.1</v>
       </c>
       <c r="D13" s="12">
-        <f>E13/150</f>
+        <f t="shared" si="0"/>
         <v>-6.371333333333333E-2</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="17">
         <v>-9.5570000000000004</v>
       </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="F13" s="10">
+        <f t="shared" si="1"/>
+        <v>-6.371333333333333E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C14" s="11">
         <v>0.12</v>
       </c>
       <c r="D14" s="12">
-        <f>E14/150</f>
+        <f t="shared" si="0"/>
         <v>-6.3513333333333324E-2</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="17">
         <v>-9.5269999999999992</v>
       </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="F14" s="10">
+        <f t="shared" si="1"/>
+        <v>-7.6215999999999983E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C15" s="11">
         <v>0.14000000000000001</v>
       </c>
       <c r="D15" s="12">
-        <f>E15/150</f>
+        <f t="shared" si="0"/>
         <v>-6.3533333333333331E-2</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="17">
         <v>-9.5299999999999994</v>
       </c>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="F15" s="10">
+        <f t="shared" si="1"/>
+        <v>-8.894666666666667E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C16" s="11">
         <v>0.16</v>
       </c>
       <c r="D16" s="12">
-        <f>E16/150</f>
+        <f t="shared" si="0"/>
         <v>-6.3479999999999995E-2</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="17">
         <v>-9.5220000000000002</v>
       </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F16" s="10">
+        <f t="shared" si="1"/>
+        <v>-1.0156799999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="11">
         <v>0.18</v>
       </c>
       <c r="D17" s="12">
-        <f>E17/150</f>
+        <f t="shared" si="0"/>
         <v>-6.3420000000000004E-2</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="17">
         <v>-9.5129999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F17" s="10">
+        <f t="shared" si="1"/>
+        <v>-1.14156E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="11">
         <v>0.2</v>
       </c>
       <c r="D18" s="12">
-        <f>E18/150</f>
+        <f t="shared" si="0"/>
         <v>-6.3126666666666664E-2</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="17">
         <v>-9.4689999999999994</v>
       </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F18" s="10">
+        <f t="shared" si="1"/>
+        <v>-1.2625333333333334E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="11">
         <v>0.22</v>
       </c>
       <c r="D19" s="12">
-        <f>E19/150</f>
+        <f t="shared" si="0"/>
         <v>-6.318E-2</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="17">
         <v>-9.4770000000000003</v>
       </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F19" s="10">
+        <f t="shared" si="1"/>
+        <v>-1.38996E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="11">
         <v>0.24</v>
       </c>
       <c r="D20" s="12">
-        <f>E20/150</f>
+        <f t="shared" si="0"/>
         <v>-6.3E-2</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="17">
         <v>-9.4499999999999993</v>
       </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F20" s="10">
+        <f t="shared" si="1"/>
+        <v>-1.512E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" s="11">
         <v>0.26</v>
       </c>
       <c r="D21" s="12">
-        <f>E21/150</f>
+        <f t="shared" si="0"/>
         <v>-6.2853333333333344E-2</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="17">
         <v>-9.4280000000000008</v>
       </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F21" s="10">
+        <f t="shared" si="1"/>
+        <v>-1.634186666666667E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" s="11">
         <v>0.28000000000000003</v>
       </c>
       <c r="D22" s="12">
-        <f>E22/150</f>
+        <f t="shared" si="0"/>
         <v>-6.2799999999999995E-2</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="17">
         <v>-9.42</v>
       </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F22" s="10">
+        <f t="shared" si="1"/>
+        <v>-1.7583999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C23" s="11">
         <v>0.3</v>
       </c>
       <c r="D23" s="12">
-        <f>E23/150</f>
+        <f t="shared" si="0"/>
         <v>-6.2366666666666667E-2</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="17">
         <v>-9.3550000000000004</v>
       </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F23" s="10">
+        <f t="shared" si="1"/>
+        <v>-1.8710000000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C24" s="11">
         <v>0.32</v>
       </c>
       <c r="D24" s="12">
-        <f>E24/150</f>
+        <f t="shared" si="0"/>
         <v>-6.2039999999999991E-2</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="17">
         <v>-9.3059999999999992</v>
       </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F24" s="10">
+        <f t="shared" si="1"/>
+        <v>-1.9852799999999997E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C25" s="11">
         <v>0.34</v>
       </c>
       <c r="D25" s="12">
-        <f>E25/150</f>
+        <f t="shared" si="0"/>
         <v>-6.1586666666666665E-2</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="17">
         <v>-9.2379999999999995</v>
       </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F25" s="10">
+        <f t="shared" si="1"/>
+        <v>-2.0939466666666667E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C26" s="11">
         <v>0.36</v>
       </c>
       <c r="D26" s="12">
-        <f>E26/150</f>
+        <f t="shared" si="0"/>
         <v>-6.132E-2</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="17">
         <v>-9.1980000000000004</v>
       </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F26" s="10">
+        <f t="shared" si="1"/>
+        <v>-2.20752E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C27" s="11">
         <v>0.38</v>
       </c>
       <c r="D27" s="12">
-        <f>E27/150</f>
+        <f t="shared" si="0"/>
         <v>-6.0773333333333332E-2</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="17">
         <v>-9.1159999999999997</v>
       </c>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F27" s="10">
+        <f t="shared" si="1"/>
+        <v>-2.3093866666666667E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C28" s="11">
         <v>0.4</v>
       </c>
       <c r="D28" s="12">
-        <f>E28/150</f>
+        <f t="shared" si="0"/>
         <v>-5.9573333333333332E-2</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E28" s="17">
         <v>-8.9359999999999999</v>
       </c>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F28" s="10">
+        <f t="shared" si="1"/>
+        <v>-2.3829333333333334E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C29" s="11">
         <v>0.42</v>
       </c>
@@ -3953,268 +4431,306 @@
         <f>E29/150</f>
         <v>-5.7846666666666664E-2</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="17">
         <v>-8.6769999999999996</v>
       </c>
-    </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F29" s="10">
+        <f t="shared" si="1"/>
+        <v>-2.4295599999999997E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C30" s="11">
         <v>0.44</v>
       </c>
       <c r="D30" s="12">
-        <f>E30/150</f>
+        <f t="shared" si="0"/>
         <v>-5.4486666666666669E-2</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="17">
         <v>-8.173</v>
       </c>
-    </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F30" s="10">
+        <f t="shared" si="1"/>
+        <v>-2.3974133333333335E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C31" s="11">
         <v>0.46</v>
       </c>
       <c r="D31" s="12">
-        <f>E31/150</f>
+        <f t="shared" si="0"/>
         <v>-4.9506666666666671E-2</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="17">
         <v>-7.4260000000000002</v>
       </c>
-    </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F31" s="10">
+        <f t="shared" si="1"/>
+        <v>-2.2773066666666671E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C32" s="11">
         <v>0.48</v>
       </c>
       <c r="D32" s="12">
-        <f>E32/150</f>
+        <f t="shared" si="0"/>
         <v>-4.0186666666666662E-2</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E32" s="17">
         <v>-6.0279999999999996</v>
       </c>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F32" s="10">
+        <f t="shared" si="1"/>
+        <v>-1.9289599999999997E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" s="11">
         <v>0.5</v>
       </c>
       <c r="D33" s="12">
-        <f>E33/150</f>
+        <f t="shared" si="0"/>
         <v>-2.3253333333333334E-2</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E33" s="17">
         <v>-3.488</v>
       </c>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F33" s="10">
+        <f t="shared" si="1"/>
+        <v>-1.1626666666666667E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C34" s="11">
         <v>0.52</v>
       </c>
       <c r="D34" s="12">
-        <f>E34/150</f>
+        <f t="shared" si="0"/>
         <v>1.1400000000000002E-3</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E34" s="17">
         <v>0.17100000000000001</v>
       </c>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F34" s="10">
+        <f t="shared" si="1"/>
+        <v>5.928000000000001E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C35" s="11">
         <v>0.54</v>
       </c>
       <c r="D35" s="12">
-        <f>E35/150</f>
+        <f t="shared" si="0"/>
         <v>4.8300000000000003E-2</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E35" s="17">
         <v>7.2450000000000001</v>
       </c>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F35" s="10">
+        <f t="shared" si="1"/>
+        <v>2.6082000000000004E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C36" s="11">
         <v>0.56000000000000005</v>
       </c>
       <c r="D36" s="12">
-        <f>E36/150</f>
+        <f t="shared" si="0"/>
         <v>9.8839999999999997E-2</v>
       </c>
-      <c r="E36" s="11">
+      <c r="E36" s="17">
         <v>14.826000000000001</v>
       </c>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F36" s="10">
+        <f t="shared" si="1"/>
+        <v>5.5350400000000001E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C37" s="11">
         <v>0.57999999999999996</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F37" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C38" s="6">
         <v>0.6</v>
       </c>
       <c r="D38" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E38" s="18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="F38" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
     </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
     </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="4"/>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="4"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="4"/>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="4"/>

</xml_diff>